<commit_message>
Added parking lot chart to second sprint backlog
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint Backlog 2.xlsx
+++ b/Sprint 2/Sprint Backlog 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/958c084b316163e4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dmail-my.sharepoint.com/personal/jsbeesla_dundee_ac_uk/Documents/Year 3/Semester 2/AC31007 - Agile Software Engineering/AC31007-AC51003-Agile-Software-Engineering---Group-1/Sprint 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD275EEB-11AE-45EB-BB92-E5C609079D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{BD275EEB-11AE-45EB-BB92-E5C609079D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDA0BE0D-3EAD-774C-A86D-BC56CD65D466}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AF66E142-1A5A-4F1D-9B0E-7F69F79079D3}"/>
+    <workbookView xWindow="38400" yWindow="2140" windowWidth="28800" windowHeight="17500" xr2:uid="{AF66E142-1A5A-4F1D-9B0E-7F69F79079D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -333,6 +333,125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3606800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F504FAE5-058F-F24A-A8B2-6A823B2020F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="3431" t="6680" r="53758" b="49456"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="279400" y="2616199"/>
+          <a:ext cx="3327400" cy="1917701"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3670300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5270500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A9FBC4F-1B94-1442-9821-1445C522CC20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3670300" y="3289300"/>
+          <a:ext cx="1600200" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2800" b="1"/>
+            <a:t>2/2/2022</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -634,24 +753,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF461105-5B91-43D0-9242-7258AC1A3E12}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="117.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="85.81640625" customWidth="1"/>
-    <col min="5" max="5" width="34.54296875" customWidth="1"/>
+    <col min="1" max="1" width="117.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="85.83203125" customWidth="1"/>
+    <col min="5" max="5" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -668,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -685,7 +804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="13"/>
       <c r="C4" s="15"/>
@@ -696,7 +815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -713,7 +832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>19</v>
       </c>
@@ -730,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="13"/>
       <c r="C7" s="15"/>
@@ -741,7 +860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="13"/>
       <c r="C8" s="15"/>
@@ -752,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="13"/>
       <c r="C9" s="15"/>
@@ -763,7 +882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
@@ -780,7 +899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="13"/>
       <c r="C11" s="15"/>
@@ -791,7 +910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -808,37 +927,37 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="18" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -847,5 +966,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>